<commit_message>
Dev hwj 1111 (#259)
* 成本信息表下载完成，总经理审批、营销部审批完成

* 问题清单720、722、723、724解决

* 成本信息数据问题修改

* 仅保存功能

* 仅保存功能开发

* 报价成本信息表问题处理

* 营销部审批，成本问题处理，报价反馈增加字段

* 报价反馈相关开发

* 报价出不来的问题解决

* 文件归档报价部分完成，报价看板问题处理

* 归档完成

---------

Co-authored-by: Zero656329 <hwj656329@163.com>
</commit_message>
<xml_diff>
--- a/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/报价审批表模板—不含样品.xlsx
+++ b/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/报价审批表模板—不含样品.xlsx
@@ -486,9 +486,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>走量(pcs)</t>
-  </si>
-  <si>
     <t>{{Sop.Year}}</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -643,6 +640,10 @@
   </si>
   <si>
     <t>报 价 审 核 表（不含样品）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际数量</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1065,7 +1066,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1254,6 +1255,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1302,16 +1315,7 @@
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2103,7 +2107,7 @@
   <dimension ref="B1:V106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+      <selection activeCell="C24" sqref="C24:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2174,20 +2178,20 @@
       <c r="M3" s="6"/>
     </row>
     <row r="4" spans="2:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
+      <c r="B4" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
@@ -2200,17 +2204,17 @@
         <v>29</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
       <c r="G5" s="42" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="2:19" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
@@ -2442,13 +2446,13 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="D19" s="63" t="s">
         <v>76</v>
-      </c>
-      <c r="D19" s="63" t="s">
-        <v>77</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="11"/>
@@ -2461,14 +2465,14 @@
       <c r="M19" s="29"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="D20" s="68" t="s">
         <v>79</v>
-      </c>
-      <c r="D20" s="87" t="s">
-        <v>80</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="11"/>
@@ -2523,23 +2527,23 @@
       <c r="M23" s="29"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="76" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="78"/>
-      <c r="E24" s="74" t="s">
+      <c r="C24" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="82"/>
+      <c r="E24" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="74" t="s">
+      <c r="F24" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="76" t="s">
+      <c r="G24" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="80" t="s">
+      <c r="H24" s="84" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="11"/>
@@ -2549,13 +2553,13 @@
       <c r="M24" s="29"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="73"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="80"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="84"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
@@ -2564,23 +2568,23 @@
     </row>
     <row r="26" spans="2:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B26" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="81" t="s">
+      <c r="D26" s="86"/>
+      <c r="E26" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="82"/>
-      <c r="E26" s="65" t="s">
+      <c r="F26" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="F26" s="66" t="s">
+      <c r="G26" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="G26" s="67" t="s">
+      <c r="H26" s="65" t="s">
         <v>73</v>
-      </c>
-      <c r="H26" s="65" t="s">
-        <v>74</v>
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -2720,23 +2724,23 @@
       <c r="B36" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="70" t="s">
+      <c r="C36" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="71"/>
+      <c r="D36" s="75"/>
       <c r="E36" s="55" t="s">
         <v>67</v>
       </c>
       <c r="F36" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="G36" s="70" t="s">
+      <c r="G36" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="H36" s="71"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="87"/>
+      <c r="J36" s="87"/>
+      <c r="K36" s="87"/>
       <c r="L36" s="16"/>
       <c r="M36" s="29"/>
     </row>
@@ -2859,48 +2863,48 @@
       <c r="O43" s="22"/>
     </row>
     <row r="44" spans="2:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="86" t="s">
+      <c r="B44" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="84" t="s">
+      <c r="C44" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="84" t="s">
+      <c r="D44" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84" t="s">
+      <c r="E44" s="69"/>
+      <c r="F44" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G44" s="84"/>
-      <c r="H44" s="84" t="s">
+      <c r="G44" s="69"/>
+      <c r="H44" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="I44" s="84"/>
-      <c r="J44" s="84" t="s">
+      <c r="I44" s="69"/>
+      <c r="J44" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="K44" s="84"/>
-      <c r="L44" s="84" t="s">
+      <c r="K44" s="69"/>
+      <c r="L44" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="M44" s="84"/>
-      <c r="N44" s="84" t="s">
+      <c r="M44" s="69"/>
+      <c r="N44" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="O44" s="84"/>
-      <c r="P44" s="84" t="s">
+      <c r="O44" s="69"/>
+      <c r="P44" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="Q44" s="84"/>
-      <c r="R44" s="84" t="s">
+      <c r="Q44" s="69"/>
+      <c r="R44" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="S44" s="85"/>
+      <c r="S44" s="70"/>
     </row>
     <row r="45" spans="2:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="86"/>
-      <c r="C45" s="84"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="69"/>
       <c r="D45" s="49" t="s">
         <v>43</v>
       </c>
@@ -3908,16 +3912,6 @@
     <row r="106" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="P44:Q44"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="J5:M5"/>
@@ -3931,6 +3925,16 @@
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="I36:K36"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="P44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dev hwj 1111 (#329)
* 成本信息表下载完成，总经理审批、营销部审批完成

* 问题清单720、722、723、724解决

* 成本信息数据问题修改

* 仅保存功能

* 仅保存功能开发

* 报价成本信息表问题处理

* 营销部审批，成本问题处理，报价反馈增加字段

* 报价反馈相关开发

* 报价出不来的问题解决

* 文件归档报价部分完成，报价看板问题处理

* 归档完成

* 梯度走量问题解决、738改变数据结构方便前端显示，756问题解决

* 客户目标价为0引发的成本问题解决，产品名改方案，梯度走量修改

* 因为汇率为空造成的异常问题解决

* 报价流程相关处理

* 报价分析看板无法显示问题处理

* 报价分析看板处理

* 审批表问题处理

* 保存优化

* 字段控制

* 增加报价方案删除接口，总经理审批二结构修改

* 归档、样品数据问题处理

* 报价策略修改，获取数据问题处理

* 产品清单逻辑修改

* 问题处理

* 线体数量、分摊率问题解决

---------

Co-authored-by: Zero656329 <hwj656329@163.com>
</commit_message>
<xml_diff>
--- a/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/报价审批表模板—不含样品.xlsx
+++ b/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/报价审批表模板—不含样品.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>报价形式：</t>
   </si>
@@ -487,10 +487,6 @@
   </si>
   <si>
     <t>{{Sop.Year}}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Sop.Motion}}</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -643,7 +639,31 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>实际数量</t>
+    <t>方案名</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>核心组件</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>型号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{QuoteCurrency}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{ProjectName}}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -776,7 +796,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -954,17 +974,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -995,17 +1004,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -1066,7 +1064,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="86">
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1225,13 +1223,13 @@
     <xf numFmtId="176" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1252,12 +1250,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1267,56 +1301,11 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2106,8 +2095,8 @@
   </sheetPr>
   <dimension ref="B1:V106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2178,20 +2167,20 @@
       <c r="M3" s="6"/>
     </row>
     <row r="4" spans="2:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
+      <c r="B4" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
@@ -2204,17 +2193,17 @@
         <v>29</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="42" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
     </row>
     <row r="6" spans="2:19" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
@@ -2384,7 +2373,9 @@
       <c r="B15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="39"/>
+      <c r="C15" s="39" t="s">
+        <v>85</v>
+      </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -2446,13 +2437,13 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="D19" s="63" t="s">
         <v>75</v>
-      </c>
-      <c r="D19" s="63" t="s">
-        <v>76</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="11"/>
@@ -2466,13 +2457,13 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="D20" s="68" t="s">
         <v>78</v>
-      </c>
-      <c r="D20" s="68" t="s">
-        <v>79</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="11"/>
@@ -2527,70 +2518,60 @@
       <c r="M23" s="29"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="82"/>
-      <c r="E24" s="78" t="s">
+      <c r="C24" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="78" t="s">
+      <c r="D24" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="80" t="s">
+      <c r="E24" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="84" t="s">
+      <c r="F24" s="79" t="s">
         <v>25</v>
       </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="29"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="29"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="77"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="79"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="78"/>
       <c r="F25" s="79"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="84"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
       <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="29"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="29"/>
     </row>
     <row r="26" spans="2:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B26" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="86"/>
-      <c r="E26" s="65" t="s">
+      <c r="D26" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="66" t="s">
+      <c r="E26" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="G26" s="67" t="s">
+      <c r="F26" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="65" t="s">
-        <v>73</v>
-      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="29"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="29"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="58"/>
@@ -2666,7 +2647,9 @@
       <c r="B32" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="17" t="s">
+        <v>86</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2707,13 +2690,23 @@
       <c r="M34" s="29"/>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B35" s="30"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="B35" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="85" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" s="84"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
@@ -2724,23 +2717,23 @@
       <c r="B36" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="74" t="s">
+      <c r="C36" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="75"/>
+      <c r="D36" s="72"/>
       <c r="E36" s="55" t="s">
         <v>67</v>
       </c>
       <c r="F36" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="G36" s="74" t="s">
+      <c r="G36" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="H36" s="75"/>
-      <c r="I36" s="87"/>
-      <c r="J36" s="87"/>
-      <c r="K36" s="87"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
       <c r="L36" s="16"/>
       <c r="M36" s="29"/>
     </row>
@@ -2863,48 +2856,48 @@
       <c r="O43" s="22"/>
     </row>
     <row r="44" spans="2:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="71" t="s">
+      <c r="B44" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="69" t="s">
+      <c r="D44" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69" t="s">
+      <c r="E44" s="81"/>
+      <c r="F44" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69" t="s">
+      <c r="G44" s="81"/>
+      <c r="H44" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="I44" s="69"/>
-      <c r="J44" s="69" t="s">
+      <c r="I44" s="81"/>
+      <c r="J44" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="K44" s="69"/>
-      <c r="L44" s="69" t="s">
+      <c r="K44" s="81"/>
+      <c r="L44" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="M44" s="69"/>
-      <c r="N44" s="69" t="s">
+      <c r="M44" s="81"/>
+      <c r="N44" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="O44" s="69"/>
-      <c r="P44" s="69" t="s">
+      <c r="O44" s="81"/>
+      <c r="P44" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="Q44" s="69"/>
-      <c r="R44" s="69" t="s">
+      <c r="Q44" s="81"/>
+      <c r="R44" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="S44" s="70"/>
+      <c r="S44" s="82"/>
     </row>
     <row r="45" spans="2:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="71"/>
-      <c r="C45" s="69"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="81"/>
       <c r="D45" s="49" t="s">
         <v>43</v>
       </c>
@@ -3911,20 +3904,7 @@
     <row r="105" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="106" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="I36:K36"/>
+  <mergeCells count="21">
     <mergeCell ref="R44:S44"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:C45"/>
@@ -3935,6 +3915,17 @@
     <mergeCell ref="L44:M44"/>
     <mergeCell ref="N44:O44"/>
     <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="I36:K36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>